<commit_message>
Documentation items and population changes
</commit_message>
<xml_diff>
--- a/Airbase_Tables.xlsx
+++ b/Airbase_Tables.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="18180" windowHeight="7680"/>
+    <workbookView xWindow="480" yWindow="36" windowWidth="18180" windowHeight="7680" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Fares" sheetId="2" r:id="rId1"/>
     <sheet name="Airport" sheetId="1" r:id="rId2"/>
     <sheet name="Flights" sheetId="3" r:id="rId3"/>
     <sheet name="Leg_Schedule" sheetId="7" r:id="rId4"/>
-    <sheet name="Flight_Fares" sheetId="4" r:id="rId5"/>
-    <sheet name="Airplane_Type" sheetId="5" r:id="rId6"/>
-    <sheet name="Airplane" sheetId="6" r:id="rId7"/>
-    <sheet name="Leg_Instance" sheetId="8" r:id="rId8"/>
-    <sheet name="Seats" sheetId="9" r:id="rId9"/>
+    <sheet name="Seats" sheetId="9" r:id="rId5"/>
+    <sheet name="Flight_Fares" sheetId="4" r:id="rId6"/>
+    <sheet name="Airplane_Type" sheetId="5" r:id="rId7"/>
+    <sheet name="Airplane" sheetId="6" r:id="rId8"/>
+    <sheet name="Leg_Instance" sheetId="8" r:id="rId9"/>
     <sheet name="Flight_Days" sheetId="10" r:id="rId10"/>
     <sheet name="Landing_Allowances" sheetId="11" r:id="rId11"/>
   </sheets>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="91">
   <si>
     <t>Table:  Airport</t>
   </si>
@@ -654,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1785,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2262,6 +2262,271 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -2432,7 +2697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2528,7 +2793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2570,7 +2835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2623,59 +2888,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>